<commit_message>
clean up files - 22 july
</commit_message>
<xml_diff>
--- a/documentation/Sense2StopDemographics.xlsx
+++ b/documentation/Sense2StopDemographics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariannemenictas/Dropbox/Postdoc_Harvard/S2S_primary_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariannemenictas/Dropbox/Postdoc_Harvard/S2S_primary_analysis/github_repository/S2S_primary_analysis/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1168F297-DE35-5E45-AD45-B90813E65C50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B9351C-9F76-9B41-94D7-330B45B080F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="27980" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="27980" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sense2StopDemographics_forMaria" sheetId="1" r:id="rId1"/>
@@ -1254,10 +1254,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1649,8 +1649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X76"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7063,8 +7063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{593EDB11-98C9-3341-9273-0B68B2D54B0D}">
   <dimension ref="A1:Y151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H63" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="X84" sqref="X84"/>
+    <sheetView topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12561,13 +12561,13 @@
         <v>0.46376811594202899</v>
       </c>
       <c r="L82" s="39"/>
-      <c r="M82" s="54" t="s">
+      <c r="M82" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="N82" s="54"/>
-      <c r="O82" s="54"/>
-      <c r="P82" s="54"/>
-      <c r="Q82" s="54"/>
+      <c r="N82" s="53"/>
+      <c r="O82" s="53"/>
+      <c r="P82" s="53"/>
+      <c r="Q82" s="53"/>
       <c r="R82" s="39"/>
       <c r="S82" s="39"/>
       <c r="T82" s="39"/>
@@ -12594,13 +12594,13 @@
         <v>0.53623188405797106</v>
       </c>
       <c r="L83" s="39"/>
-      <c r="M83" s="53"/>
-      <c r="N83" s="54" t="s">
+      <c r="M83" s="54"/>
+      <c r="N83" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="O83" s="54"/>
-      <c r="P83" s="54"/>
-      <c r="Q83" s="54"/>
+      <c r="O83" s="53"/>
+      <c r="P83" s="53"/>
+      <c r="Q83" s="53"/>
       <c r="R83" s="40">
         <v>32</v>
       </c>
@@ -12624,13 +12624,13 @@
       <c r="H84" s="27"/>
       <c r="I84" s="28"/>
       <c r="L84" s="39"/>
-      <c r="M84" s="53"/>
-      <c r="N84" s="54" t="s">
+      <c r="M84" s="54"/>
+      <c r="N84" s="53" t="s">
         <v>144</v>
       </c>
-      <c r="O84" s="54"/>
-      <c r="P84" s="54"/>
-      <c r="Q84" s="54"/>
+      <c r="O84" s="53"/>
+      <c r="P84" s="53"/>
+      <c r="Q84" s="53"/>
       <c r="R84" s="40">
         <v>37</v>
       </c>
@@ -12665,13 +12665,13 @@
         <v>2.8985507246376812E-2</v>
       </c>
       <c r="L85" s="39"/>
-      <c r="M85" s="54" t="s">
+      <c r="M85" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="N85" s="54"/>
-      <c r="O85" s="54"/>
-      <c r="P85" s="54"/>
-      <c r="Q85" s="54"/>
+      <c r="N85" s="53"/>
+      <c r="O85" s="53"/>
+      <c r="P85" s="53"/>
+      <c r="Q85" s="53"/>
       <c r="R85" s="39"/>
       <c r="S85" s="39"/>
       <c r="T85" s="42"/>
@@ -12698,13 +12698,13 @@
         <v>0.56521739130434778</v>
       </c>
       <c r="L86" s="39"/>
-      <c r="M86" s="53"/>
-      <c r="N86" s="54" t="s">
+      <c r="M86" s="54"/>
+      <c r="N86" s="53" t="s">
         <v>145</v>
       </c>
-      <c r="O86" s="54"/>
-      <c r="P86" s="54"/>
-      <c r="Q86" s="54"/>
+      <c r="O86" s="53"/>
+      <c r="P86" s="53"/>
+      <c r="Q86" s="53"/>
       <c r="R86" s="40">
         <v>2</v>
       </c>
@@ -12737,13 +12737,13 @@
         <v>0.2608695652173913</v>
       </c>
       <c r="L87" s="39"/>
-      <c r="M87" s="53"/>
-      <c r="N87" s="54" t="s">
+      <c r="M87" s="54"/>
+      <c r="N87" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="O87" s="54"/>
-      <c r="P87" s="54"/>
-      <c r="Q87" s="54"/>
+      <c r="O87" s="53"/>
+      <c r="P87" s="53"/>
+      <c r="Q87" s="53"/>
       <c r="R87" s="40">
         <v>39</v>
       </c>
@@ -12776,13 +12776,13 @@
         <v>8.6956521739130432E-2</v>
       </c>
       <c r="L88" s="39"/>
-      <c r="M88" s="53"/>
-      <c r="N88" s="54" t="s">
+      <c r="M88" s="54"/>
+      <c r="N88" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="O88" s="54"/>
-      <c r="P88" s="54"/>
-      <c r="Q88" s="54"/>
+      <c r="O88" s="53"/>
+      <c r="P88" s="53"/>
+      <c r="Q88" s="53"/>
       <c r="R88" s="40">
         <v>18</v>
       </c>
@@ -12815,13 +12815,13 @@
         <v>5.7971014492753624E-2</v>
       </c>
       <c r="L89" s="39"/>
-      <c r="M89" s="53"/>
-      <c r="N89" s="54" t="s">
+      <c r="M89" s="54"/>
+      <c r="N89" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="O89" s="54"/>
-      <c r="P89" s="54"/>
-      <c r="Q89" s="54"/>
+      <c r="O89" s="53"/>
+      <c r="P89" s="53"/>
+      <c r="Q89" s="53"/>
       <c r="R89" s="40">
         <v>10</v>
       </c>
@@ -12846,13 +12846,13 @@
       <c r="H90" s="27"/>
       <c r="I90" s="28"/>
       <c r="L90" s="39"/>
-      <c r="M90" s="54" t="s">
+      <c r="M90" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="N90" s="54"/>
-      <c r="O90" s="54"/>
-      <c r="P90" s="54"/>
-      <c r="Q90" s="54"/>
+      <c r="N90" s="53"/>
+      <c r="O90" s="53"/>
+      <c r="P90" s="53"/>
+      <c r="Q90" s="53"/>
       <c r="R90" s="40"/>
       <c r="S90" s="40"/>
       <c r="T90" s="41"/>
@@ -12881,13 +12881,13 @@
         <v>0.87142857142857144</v>
       </c>
       <c r="L91" s="39"/>
-      <c r="M91" s="53"/>
-      <c r="N91" s="54" t="s">
+      <c r="M91" s="54"/>
+      <c r="N91" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="O91" s="54"/>
-      <c r="P91" s="54"/>
-      <c r="Q91" s="54"/>
+      <c r="O91" s="53"/>
+      <c r="P91" s="53"/>
+      <c r="Q91" s="53"/>
       <c r="R91" s="40">
         <v>1</v>
       </c>
@@ -12920,13 +12920,13 @@
         <v>0.11428571428571428</v>
       </c>
       <c r="L92" s="39"/>
-      <c r="M92" s="53"/>
-      <c r="N92" s="54" t="s">
+      <c r="M92" s="54"/>
+      <c r="N92" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="O92" s="54"/>
-      <c r="P92" s="54"/>
-      <c r="Q92" s="54"/>
+      <c r="O92" s="53"/>
+      <c r="P92" s="53"/>
+      <c r="Q92" s="53"/>
       <c r="R92" s="40">
         <v>4</v>
       </c>
@@ -12950,13 +12950,13 @@
       <c r="H93" s="27"/>
       <c r="I93" s="28"/>
       <c r="L93" s="39"/>
-      <c r="M93" s="53"/>
-      <c r="N93" s="54" t="s">
+      <c r="M93" s="54"/>
+      <c r="N93" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="O93" s="54"/>
-      <c r="P93" s="54"/>
-      <c r="Q93" s="54"/>
+      <c r="O93" s="53"/>
+      <c r="P93" s="53"/>
+      <c r="Q93" s="53"/>
       <c r="R93" s="40">
         <v>17</v>
       </c>
@@ -12991,13 +12991,13 @@
         <v>1.4492753623188406E-2</v>
       </c>
       <c r="L94" s="39"/>
-      <c r="M94" s="53"/>
-      <c r="N94" s="54" t="s">
+      <c r="M94" s="54"/>
+      <c r="N94" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="O94" s="54"/>
-      <c r="P94" s="54"/>
-      <c r="Q94" s="54"/>
+      <c r="O94" s="53"/>
+      <c r="P94" s="53"/>
+      <c r="Q94" s="53"/>
       <c r="R94" s="40">
         <v>23</v>
       </c>
@@ -13030,13 +13030,13 @@
         <v>5.7971014492753624E-2</v>
       </c>
       <c r="L95" s="39"/>
-      <c r="M95" s="53"/>
-      <c r="N95" s="54" t="s">
+      <c r="M95" s="54"/>
+      <c r="N95" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="O95" s="54"/>
-      <c r="P95" s="54"/>
-      <c r="Q95" s="54"/>
+      <c r="O95" s="53"/>
+      <c r="P95" s="53"/>
+      <c r="Q95" s="53"/>
       <c r="R95" s="40">
         <v>9</v>
       </c>
@@ -13069,13 +13069,13 @@
         <v>0.24637681159420291</v>
       </c>
       <c r="L96" s="39"/>
-      <c r="M96" s="53"/>
-      <c r="N96" s="54" t="s">
+      <c r="M96" s="54"/>
+      <c r="N96" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="O96" s="54"/>
-      <c r="P96" s="54"/>
-      <c r="Q96" s="54"/>
+      <c r="O96" s="53"/>
+      <c r="P96" s="53"/>
+      <c r="Q96" s="53"/>
       <c r="R96" s="40">
         <v>8</v>
       </c>
@@ -13108,13 +13108,13 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="L97" s="39"/>
-      <c r="M97" s="53"/>
-      <c r="N97" s="54" t="s">
+      <c r="M97" s="54"/>
+      <c r="N97" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="O97" s="54"/>
-      <c r="P97" s="54"/>
-      <c r="Q97" s="54"/>
+      <c r="O97" s="53"/>
+      <c r="P97" s="53"/>
+      <c r="Q97" s="53"/>
       <c r="R97" s="40">
         <v>6</v>
       </c>
@@ -13148,13 +13148,13 @@
         <v>0.13043478260869565</v>
       </c>
       <c r="L98" s="39"/>
-      <c r="M98" s="54" t="s">
+      <c r="M98" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="N98" s="54"/>
-      <c r="O98" s="54"/>
-      <c r="P98" s="54"/>
-      <c r="Q98" s="54"/>
+      <c r="N98" s="53"/>
+      <c r="O98" s="53"/>
+      <c r="P98" s="53"/>
+      <c r="Q98" s="53"/>
       <c r="R98" s="40"/>
       <c r="S98" s="40"/>
       <c r="T98" s="41"/>
@@ -13181,7 +13181,7 @@
         <v>0.11594202898550725</v>
       </c>
       <c r="L99" s="39"/>
-      <c r="M99" s="53"/>
+      <c r="M99" s="54"/>
       <c r="N99" s="48" t="s">
         <v>103</v>
       </c>
@@ -13220,7 +13220,7 @@
         <v>0</v>
       </c>
       <c r="L100" s="39"/>
-      <c r="M100" s="53"/>
+      <c r="M100" s="54"/>
       <c r="N100" s="48" t="s">
         <v>104</v>
       </c>
@@ -13259,7 +13259,7 @@
         <v>2.8985507246376812E-2</v>
       </c>
       <c r="L101" s="39"/>
-      <c r="M101" s="53"/>
+      <c r="M101" s="54"/>
       <c r="N101" s="48" t="s">
         <v>105</v>
       </c>
@@ -13298,13 +13298,13 @@
         <v>2.8985507246376812E-2</v>
       </c>
       <c r="L102" s="39"/>
-      <c r="M102" s="53"/>
-      <c r="N102" s="54" t="s">
+      <c r="M102" s="54"/>
+      <c r="N102" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="O102" s="54"/>
-      <c r="P102" s="54"/>
-      <c r="Q102" s="54"/>
+      <c r="O102" s="53"/>
+      <c r="P102" s="53"/>
+      <c r="Q102" s="53"/>
       <c r="R102" s="40">
         <v>5</v>
       </c>
@@ -13328,13 +13328,13 @@
       <c r="H103" s="27"/>
       <c r="I103" s="28"/>
       <c r="L103" s="39"/>
-      <c r="M103" s="53"/>
-      <c r="N103" s="54" t="s">
+      <c r="M103" s="54"/>
+      <c r="N103" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="O103" s="54"/>
-      <c r="P103" s="54"/>
-      <c r="Q103" s="54"/>
+      <c r="O103" s="53"/>
+      <c r="P103" s="53"/>
+      <c r="Q103" s="53"/>
       <c r="R103" s="40">
         <v>7</v>
       </c>
@@ -13369,13 +13369,13 @@
         <v>0.39130434782608697</v>
       </c>
       <c r="L104" s="39"/>
-      <c r="M104" s="54" t="s">
+      <c r="M104" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="N104" s="54"/>
-      <c r="O104" s="54"/>
-      <c r="P104" s="54"/>
-      <c r="Q104" s="54"/>
+      <c r="N104" s="53"/>
+      <c r="O104" s="53"/>
+      <c r="P104" s="53"/>
+      <c r="Q104" s="53"/>
       <c r="R104" s="50"/>
       <c r="S104" s="50"/>
       <c r="T104" s="50"/>
@@ -13402,7 +13402,7 @@
         <v>0.21739130434782608</v>
       </c>
       <c r="L105" s="39"/>
-      <c r="M105" s="53"/>
+      <c r="M105" s="54"/>
       <c r="N105" s="48" t="s">
         <v>109</v>
       </c>
@@ -13441,7 +13441,7 @@
         <v>0.21739130434782608</v>
       </c>
       <c r="L106" s="39"/>
-      <c r="M106" s="53"/>
+      <c r="M106" s="54"/>
       <c r="N106" s="48" t="s">
         <v>108</v>
       </c>
@@ -13480,7 +13480,7 @@
         <v>7.2463768115942032E-2</v>
       </c>
       <c r="L107" s="39"/>
-      <c r="M107" s="53"/>
+      <c r="M107" s="54"/>
       <c r="N107" s="48" t="s">
         <v>110</v>
       </c>
@@ -13519,13 +13519,13 @@
         <v>0.10144927536231885</v>
       </c>
       <c r="L108" s="39"/>
-      <c r="M108" s="53"/>
-      <c r="N108" s="54" t="s">
+      <c r="M108" s="54"/>
+      <c r="N108" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="O108" s="54"/>
-      <c r="P108" s="54"/>
-      <c r="Q108" s="54"/>
+      <c r="O108" s="53"/>
+      <c r="P108" s="53"/>
+      <c r="Q108" s="53"/>
       <c r="R108" s="40">
         <v>5</v>
       </c>
@@ -13549,13 +13549,13 @@
       <c r="H109" s="27"/>
       <c r="I109" s="28"/>
       <c r="L109" s="39"/>
-      <c r="M109" s="53"/>
-      <c r="N109" s="54" t="s">
+      <c r="M109" s="54"/>
+      <c r="N109" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="O109" s="54"/>
-      <c r="P109" s="54"/>
-      <c r="Q109" s="54"/>
+      <c r="O109" s="53"/>
+      <c r="P109" s="53"/>
+      <c r="Q109" s="53"/>
       <c r="R109" s="40">
         <v>2</v>
       </c>
@@ -13590,13 +13590,13 @@
         <v>0.71014492753623193</v>
       </c>
       <c r="L110" s="39"/>
-      <c r="M110" s="54" t="s">
+      <c r="M110" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="N110" s="54"/>
-      <c r="O110" s="54"/>
-      <c r="P110" s="54"/>
-      <c r="Q110" s="54"/>
+      <c r="N110" s="53"/>
+      <c r="O110" s="53"/>
+      <c r="P110" s="53"/>
+      <c r="Q110" s="53"/>
       <c r="R110" s="50"/>
       <c r="S110" s="50"/>
       <c r="T110" s="50"/>
@@ -13623,7 +13623,7 @@
         <v>0.14492753623188406</v>
       </c>
       <c r="L111" s="39"/>
-      <c r="M111" s="53"/>
+      <c r="M111" s="54"/>
       <c r="N111" s="48" t="s">
         <v>115</v>
       </c>
@@ -13662,7 +13662,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
       <c r="L112" s="39"/>
-      <c r="M112" s="53"/>
+      <c r="M112" s="54"/>
       <c r="N112" s="48" t="s">
         <v>116</v>
       </c>
@@ -13701,13 +13701,13 @@
         <v>7.2463768115942032E-2</v>
       </c>
       <c r="L113" s="39"/>
-      <c r="M113" s="53"/>
-      <c r="N113" s="54" t="s">
+      <c r="M113" s="54"/>
+      <c r="N113" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="O113" s="54"/>
-      <c r="P113" s="54"/>
-      <c r="Q113" s="54"/>
+      <c r="O113" s="53"/>
+      <c r="P113" s="53"/>
+      <c r="Q113" s="53"/>
       <c r="R113" s="40">
         <v>4</v>
       </c>
@@ -13740,13 +13740,13 @@
         <v>2.8985507246376812E-2</v>
       </c>
       <c r="L114" s="39"/>
-      <c r="M114" s="53"/>
-      <c r="N114" s="54" t="s">
+      <c r="M114" s="54"/>
+      <c r="N114" s="53" t="s">
         <v>118</v>
       </c>
-      <c r="O114" s="54"/>
-      <c r="P114" s="54"/>
-      <c r="Q114" s="54"/>
+      <c r="O114" s="53"/>
+      <c r="P114" s="53"/>
+      <c r="Q114" s="53"/>
       <c r="R114" s="40">
         <v>59</v>
       </c>
@@ -13770,13 +13770,13 @@
       <c r="H115" s="27"/>
       <c r="I115" s="28"/>
       <c r="L115" s="39"/>
-      <c r="M115" s="54" t="s">
+      <c r="M115" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="N115" s="54"/>
-      <c r="O115" s="54"/>
-      <c r="P115" s="54"/>
-      <c r="Q115" s="54"/>
+      <c r="N115" s="53"/>
+      <c r="O115" s="53"/>
+      <c r="P115" s="53"/>
+      <c r="Q115" s="53"/>
       <c r="R115" s="50"/>
       <c r="S115" s="50"/>
       <c r="T115" s="50"/>
@@ -13806,12 +13806,12 @@
       </c>
       <c r="L116" s="39"/>
       <c r="M116" s="49"/>
-      <c r="N116" s="54" t="s">
+      <c r="N116" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="O116" s="54"/>
-      <c r="P116" s="54"/>
-      <c r="Q116" s="54"/>
+      <c r="O116" s="53"/>
+      <c r="P116" s="53"/>
+      <c r="Q116" s="53"/>
       <c r="R116" s="40">
         <v>44</v>
       </c>
@@ -13845,12 +13845,12 @@
       </c>
       <c r="L117" s="39"/>
       <c r="M117" s="50"/>
-      <c r="N117" s="54" t="s">
+      <c r="N117" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="O117" s="54"/>
-      <c r="P117" s="54"/>
-      <c r="Q117" s="54"/>
+      <c r="O117" s="53"/>
+      <c r="P117" s="53"/>
+      <c r="Q117" s="53"/>
       <c r="R117" s="40">
         <v>24</v>
       </c>
@@ -14191,13 +14191,13 @@
         <v>70</v>
       </c>
       <c r="L126" s="39"/>
-      <c r="M126" s="54" t="s">
+      <c r="M126" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="N126" s="54"/>
-      <c r="O126" s="54"/>
-      <c r="P126" s="54"/>
-      <c r="Q126" s="54"/>
+      <c r="N126" s="53"/>
+      <c r="O126" s="53"/>
+      <c r="P126" s="53"/>
+      <c r="Q126" s="53"/>
       <c r="R126" s="43">
         <v>30.14314952876645</v>
       </c>
@@ -14490,6 +14490,9 @@
     <mergeCell ref="N84:Q84"/>
     <mergeCell ref="N83:Q83"/>
     <mergeCell ref="N91:Q91"/>
+    <mergeCell ref="M91:M97"/>
+    <mergeCell ref="N96:Q96"/>
+    <mergeCell ref="N95:Q95"/>
     <mergeCell ref="M111:M114"/>
     <mergeCell ref="M127:Q127"/>
     <mergeCell ref="M126:Q126"/>
@@ -14506,14 +14509,11 @@
     <mergeCell ref="N109:Q109"/>
     <mergeCell ref="N102:Q102"/>
     <mergeCell ref="N103:Q103"/>
-    <mergeCell ref="M91:M97"/>
     <mergeCell ref="M98:Q98"/>
     <mergeCell ref="M104:Q104"/>
     <mergeCell ref="M105:M109"/>
     <mergeCell ref="M99:M103"/>
     <mergeCell ref="N97:Q97"/>
-    <mergeCell ref="N96:Q96"/>
-    <mergeCell ref="N95:Q95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -14542,8 +14542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:D22"/>
+    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>